<commit_message>
modify SLG building config
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/BB_Build.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/BB_Build.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NF\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,10 +42,6 @@
     <t>Func1</t>
   </si>
   <si>
-    <t>COC_Resources/animation/building/altar/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Build_Altar_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -54,55 +50,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/arena/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Build_Camp_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/camp/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Build_Gold_Mine_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/gold_mine/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Build_Item_Hourse_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/item_hourse/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Build_League_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/league/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Build_Magic_Hourse_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/magic_hourse/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Build_Tower_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/tower/1.prefab</t>
+    <t>Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级祭坛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级竞技场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级兵营</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级金矿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级道具屋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级公会</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级魔法屋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级箭塔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级大厅</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -110,47 +118,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>COC_Resources/animation/building/town/1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级祭坛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级竞技场</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级兵营</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级金矿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级道具屋</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级公会</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级魔法屋</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级箭塔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一级大厅</t>
+    <t>Prefabs/Object/Town_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Tower_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Item_hourse_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/MagicHourse_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/League_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/GoldMine_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Camp_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Arena_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Altar_1_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,7 +551,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -596,12 +596,12 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -619,12 +619,12 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -633,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -642,12 +642,12 @@
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -656,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -665,12 +665,12 @@
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -688,12 +688,12 @@
         <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -702,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
@@ -711,12 +711,12 @@
         <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -734,12 +734,12 @@
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>6</v>
@@ -757,12 +757,12 @@
         <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -771,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
@@ -780,12 +780,12 @@
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -794,16 +794,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove Gamelogic project, modify SLG building config
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/BB_Build.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/BB_Build.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -118,39 +118,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Icon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShowName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Altar_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Func1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Altar_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Arena_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arena_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Camp_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camp_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/GoldMine_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoldMine_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Item_hourse_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item_hourse_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/League_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>League_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/MagicHourse_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MagicHourse_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Object/Tower_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tower_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Prefabs/Object/Town_1_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Object/Tower_1_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Object/Item_hourse_1_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Object/MagicHourse_1_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Object/League_1_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Object/GoldMine_1_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Object/Camp_1_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Object/Arena_1_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Object/Altar_1_1</t>
+    <t>Town_1_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -562,8 +610,7 @@
     <col min="4" max="4" width="59.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="12.75" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="7" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="16.875" customWidth="1"/>
     <col min="11" max="11" width="14.625" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
@@ -576,7 +623,7 @@
     <col min="20" max="20" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,10 +643,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -610,19 +663,25 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -633,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -642,10 +701,16 @@
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -656,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -665,10 +730,16 @@
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -679,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -688,10 +759,16 @@
         <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -702,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
@@ -711,10 +788,16 @@
         <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -725,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -734,10 +817,16 @@
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -748,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>6</v>
@@ -757,10 +846,16 @@
         <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -771,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
@@ -780,10 +875,16 @@
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -794,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
@@ -803,6 +904,12 @@
         <v>6</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dev-> merge ini, struct----test
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/BB_Build.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/BB_Build.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="19455" windowHeight="9990"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Property1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -201,12 +201,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -227,11 +227,55 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -241,6 +285,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -249,51 +294,31 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,83 +334,51 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,25 +399,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,157 +531,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,24 +694,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -737,8 +706,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,6 +727,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -773,17 +766,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -792,152 +779,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,25 +940,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1397,207 +1381,207 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:9">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:9">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9" t="b">
+      <c r="B3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:9">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9" t="b">
+      <c r="B4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:9">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="9" t="b">
+      <c r="B5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:9">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9" t="b">
+      <c r="B6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" ht="14.25" spans="1:9">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B8">
@@ -1606,27 +1590,27 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B9">
@@ -1635,27 +1619,27 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B10">
@@ -1664,56 +1648,56 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B12">
@@ -1722,27 +1706,27 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B13">
@@ -1751,27 +1735,27 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B14">
@@ -1780,27 +1764,27 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B15">
@@ -1809,27 +1793,27 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B16">
@@ -1838,22 +1822,22 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>